<commit_message>
GUI Meeting and Sample tkinter
</commit_message>
<xml_diff>
--- a/Library.xlsx
+++ b/Library.xlsx
@@ -24,9 +24,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -82192,7 +82193,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n"/>
+      <c r="A3" s="8" t="n"/>
       <c r="B3" s="8" t="n">
         <v>1192</v>
       </c>
@@ -82209,7 +82210,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="n"/>
+      <c r="A4" s="8" t="n"/>
       <c r="B4" s="8" t="n">
         <v>1399</v>
       </c>
@@ -82245,7 +82246,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="n"/>
+      <c r="A6" s="8" t="n"/>
       <c r="B6" s="8" t="n">
         <v>3220</v>
       </c>
@@ -82338,7 +82339,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="n"/>
+      <c r="A11" s="8" t="n"/>
       <c r="B11" s="8" t="n">
         <v>511</v>
       </c>
@@ -82488,7 +82489,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="n"/>
+      <c r="A19" s="8" t="n"/>
       <c r="B19" s="8" t="n">
         <v>2098</v>
       </c>
@@ -82524,7 +82525,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="n"/>
+      <c r="A21" s="8" t="n"/>
       <c r="B21" s="8" t="n">
         <v>859</v>
       </c>
@@ -83206,7 +83207,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="11" t="n"/>
+      <c r="A57" s="8" t="n"/>
       <c r="B57" s="8" t="n">
         <v>2827</v>
       </c>
@@ -83223,7 +83224,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="12" t="n"/>
+      <c r="A58" s="8" t="n"/>
       <c r="B58" s="8" t="n">
         <v>766</v>
       </c>
@@ -83962,7 +83963,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="12" t="n"/>
+      <c r="A97" s="8" t="n"/>
       <c r="B97" s="8" t="n">
         <v>2842</v>
       </c>
@@ -84017,7 +84018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -84052,13 +84053,13 @@
         <v>1160</v>
       </c>
       <c r="B2" t="n">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="3">
@@ -84066,13 +84067,13 @@
         <v>1271</v>
       </c>
       <c r="B3" t="n">
-        <v>5.850000000000001</v>
+        <v>5.95</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>5.850000000000001</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="4">
@@ -84080,13 +84081,13 @@
         <v>1289</v>
       </c>
       <c r="B4" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="5">
@@ -84094,13 +84095,13 @@
         <v>1331</v>
       </c>
       <c r="B5" t="n">
-        <v>5.95</v>
+        <v>6.050000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>5.95</v>
+        <v>6.050000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -84108,13 +84109,13 @@
         <v>1340</v>
       </c>
       <c r="B6" t="n">
-        <v>8.699999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>8.699999999999999</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="7">
@@ -84122,13 +84123,13 @@
         <v>1343</v>
       </c>
       <c r="B7" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="8">
@@ -84136,13 +84137,13 @@
         <v>1370</v>
       </c>
       <c r="B8" t="n">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="9">
@@ -84150,13 +84151,13 @@
         <v>1394</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -84164,13 +84165,13 @@
         <v>1406</v>
       </c>
       <c r="B10" t="n">
-        <v>5.45</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.45</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -84178,13 +84179,13 @@
         <v>1454</v>
       </c>
       <c r="B11" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="12">
@@ -84192,13 +84193,13 @@
         <v>1502</v>
       </c>
       <c r="B12" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -84206,13 +84207,13 @@
         <v>1508</v>
       </c>
       <c r="B13" t="n">
-        <v>8.65</v>
+        <v>8.850000000000001</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>8.65</v>
+        <v>8.850000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -84220,13 +84221,13 @@
         <v>1553</v>
       </c>
       <c r="B14" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="15">
@@ -84234,13 +84235,13 @@
         <v>1574</v>
       </c>
       <c r="B15" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="16">
@@ -84248,13 +84249,13 @@
         <v>1577</v>
       </c>
       <c r="B16" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="17">
@@ -84262,13 +84263,13 @@
         <v>1763</v>
       </c>
       <c r="B17" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -84276,13 +84277,13 @@
         <v>1787</v>
       </c>
       <c r="B18" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="19">
@@ -84290,13 +84291,13 @@
         <v>1799</v>
       </c>
       <c r="B19" t="n">
-        <v>5.45</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.45</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -84304,13 +84305,13 @@
         <v>1856</v>
       </c>
       <c r="B20" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="21">
@@ -84318,13 +84319,13 @@
         <v>1862</v>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="22">
@@ -84332,13 +84333,13 @@
         <v>1940</v>
       </c>
       <c r="B22" t="n">
-        <v>6.350000000000001</v>
+        <v>6.45</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6.350000000000001</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="23">
@@ -84346,13 +84347,13 @@
         <v>2009</v>
       </c>
       <c r="B23" t="n">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="24">
@@ -84360,13 +84361,13 @@
         <v>2039</v>
       </c>
       <c r="B24" t="n">
-        <v>6.050000000000001</v>
+        <v>6.15</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6.050000000000001</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="25">
@@ -84374,13 +84375,13 @@
         <v>2090</v>
       </c>
       <c r="B25" t="n">
-        <v>6.2</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6.2</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -84388,13 +84389,13 @@
         <v>2141</v>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -84402,13 +84403,13 @@
         <v>2150</v>
       </c>
       <c r="B27" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="28">
@@ -84416,13 +84417,13 @@
         <v>2156</v>
       </c>
       <c r="B28" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="29">
@@ -84430,13 +84431,13 @@
         <v>2162</v>
       </c>
       <c r="B29" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="30">
@@ -84444,13 +84445,13 @@
         <v>2204</v>
       </c>
       <c r="B30" t="n">
-        <v>5.800000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>5.800000000000001</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="31">
@@ -84458,13 +84459,13 @@
         <v>2207</v>
       </c>
       <c r="B31" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="32">
@@ -84472,13 +84473,13 @@
         <v>2216</v>
       </c>
       <c r="B32" t="n">
-        <v>6.300000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.300000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="33">
@@ -84486,13 +84487,13 @@
         <v>2237</v>
       </c>
       <c r="B33" t="n">
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="34">
@@ -84500,13 +84501,13 @@
         <v>2258</v>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -84514,13 +84515,13 @@
         <v>2336</v>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="36">
@@ -84528,13 +84529,13 @@
         <v>2363</v>
       </c>
       <c r="B36" t="n">
-        <v>5.800000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>5.800000000000001</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="37">
@@ -84542,13 +84543,13 @@
         <v>2402</v>
       </c>
       <c r="B37" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="38">
@@ -84556,13 +84557,13 @@
         <v>2498</v>
       </c>
       <c r="B38" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="39">
@@ -84570,13 +84571,13 @@
         <v>2543</v>
       </c>
       <c r="B39" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="40">
@@ -84584,13 +84585,13 @@
         <v>2639</v>
       </c>
       <c r="B40" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="41">
@@ -84598,13 +84599,13 @@
         <v>2651</v>
       </c>
       <c r="B41" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="42">
@@ -84612,13 +84613,13 @@
         <v>2657</v>
       </c>
       <c r="B42" t="n">
-        <v>4.850000000000001</v>
+        <v>4.95</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>4.850000000000001</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="43">
@@ -84626,13 +84627,13 @@
         <v>2747</v>
       </c>
       <c r="B43" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -84640,13 +84641,13 @@
         <v>2798</v>
       </c>
       <c r="B44" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -84654,13 +84655,13 @@
         <v>2819</v>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="46">
@@ -84668,13 +84669,13 @@
         <v>2951</v>
       </c>
       <c r="B46" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -84682,13 +84683,13 @@
         <v>2972</v>
       </c>
       <c r="B47" t="n">
-        <v>4.5</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.5</v>
+        <v>4.600000000000001</v>
       </c>
     </row>
     <row r="48">
@@ -84696,13 +84697,13 @@
         <v>2975</v>
       </c>
       <c r="B48" t="n">
-        <v>9.699999999999999</v>
+        <v>10</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>9.699999999999999</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49">
@@ -84710,13 +84711,13 @@
         <v>2990</v>
       </c>
       <c r="B49" t="n">
-        <v>4.350000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4.350000000000001</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="50">
@@ -84724,13 +84725,13 @@
         <v>3053</v>
       </c>
       <c r="B50" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="51">
@@ -84738,13 +84739,13 @@
         <v>3074</v>
       </c>
       <c r="B51" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -84752,13 +84753,13 @@
         <v>3104</v>
       </c>
       <c r="B52" t="n">
-        <v>4.600000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>4.600000000000001</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="53">
@@ -84766,13 +84767,13 @@
         <v>3146</v>
       </c>
       <c r="B53" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>5.550000000000001</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="54">
@@ -84780,13 +84781,13 @@
         <v>3230</v>
       </c>
       <c r="B54" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="55">
@@ -84794,13 +84795,13 @@
         <v>3242</v>
       </c>
       <c r="B55" t="n">
-        <v>4.7</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.7</v>
+        <v>4.800000000000001</v>
       </c>
     </row>
     <row r="56">
@@ -84808,13 +84809,13 @@
         <v>3245</v>
       </c>
       <c r="B56" t="n">
-        <v>6.300000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6.300000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="57">
@@ -84822,13 +84823,13 @@
         <v>3269</v>
       </c>
       <c r="B57" t="n">
-        <v>4.800000000000001</v>
+        <v>4.9</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>4.800000000000001</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="58">
@@ -84836,13 +84837,13 @@
         <v>3362</v>
       </c>
       <c r="B58" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="59">
@@ -84850,13 +84851,13 @@
         <v>3479</v>
       </c>
       <c r="B59" t="n">
-        <v>4.75</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4.75</v>
+        <v>4.850000000000001</v>
       </c>
     </row>
     <row r="60">
@@ -84864,13 +84865,13 @@
         <v>3503</v>
       </c>
       <c r="B60" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -84878,13 +84879,13 @@
         <v>3539</v>
       </c>
       <c r="B61" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="62">
@@ -84892,13 +84893,13 @@
         <v>3608</v>
       </c>
       <c r="B62" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>5.75</v>
+        <v>5.850000000000001</v>
       </c>
     </row>
     <row r="63">
@@ -84906,13 +84907,13 @@
         <v>3647</v>
       </c>
       <c r="B63" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="64">
@@ -84920,13 +84921,13 @@
         <v>3653</v>
       </c>
       <c r="B64" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="65">
@@ -84934,13 +84935,13 @@
         <v>3671</v>
       </c>
       <c r="B65" t="n">
-        <v>4.95</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>4.95</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="66">
@@ -84948,13 +84949,13 @@
         <v>3680</v>
       </c>
       <c r="B66" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="67">
@@ -84962,13 +84963,13 @@
         <v>3683</v>
       </c>
       <c r="B67" t="n">
-        <v>6.2</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>6.2</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="68">
@@ -84976,13 +84977,13 @@
         <v>3722</v>
       </c>
       <c r="B68" t="n">
-        <v>4.100000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>4.100000000000001</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="69">
@@ -84990,13 +84991,13 @@
         <v>3728</v>
       </c>
       <c r="B69" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="70">
@@ -85004,13 +85005,13 @@
         <v>3749</v>
       </c>
       <c r="B70" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -85018,13 +85019,13 @@
         <v>3773</v>
       </c>
       <c r="B71" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="72">
@@ -85032,13 +85033,13 @@
         <v>3794</v>
       </c>
       <c r="B72" t="n">
-        <v>3.55</v>
+        <v>3.65</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>3.55</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="73">
@@ -85046,13 +85047,13 @@
         <v>3800</v>
       </c>
       <c r="B73" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="74">
@@ -85060,13 +85061,13 @@
         <v>3803</v>
       </c>
       <c r="B74" t="n">
-        <v>3.55</v>
+        <v>3.65</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3.55</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="75">
@@ -85074,13 +85075,13 @@
         <v>3821</v>
       </c>
       <c r="B75" t="n">
-        <v>5.850000000000001</v>
+        <v>5.95</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>5.850000000000001</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="76">
@@ -85088,13 +85089,13 @@
         <v>3824</v>
       </c>
       <c r="B76" t="n">
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="77">
@@ -85102,13 +85103,13 @@
         <v>3866</v>
       </c>
       <c r="B77" t="n">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="78">
@@ -85116,13 +85117,13 @@
         <v>3923</v>
       </c>
       <c r="B78" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>6.25</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -85130,13 +85131,13 @@
         <v>3932</v>
       </c>
       <c r="B79" t="n">
-        <v>4.25</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>4.25</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -85144,13 +85145,13 @@
         <v>3959</v>
       </c>
       <c r="B80" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>5.100000000000001</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="81">
@@ -85158,13 +85159,13 @@
         <v>3968</v>
       </c>
       <c r="B81" t="n">
-        <v>5.95</v>
+        <v>6.050000000000001</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>5.95</v>
+        <v>6.050000000000001</v>
       </c>
     </row>
     <row r="82">
@@ -85172,13 +85173,13 @@
         <v>3977</v>
       </c>
       <c r="B82" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="83">
@@ -85186,13 +85187,13 @@
         <v>3980</v>
       </c>
       <c r="B83" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>5.350000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="84">
@@ -85200,13 +85201,13 @@
         <v>3986</v>
       </c>
       <c r="B84" t="n">
-        <v>4.5</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>4.5</v>
+        <v>4.600000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -85214,13 +85215,13 @@
         <v>3989</v>
       </c>
       <c r="B85" t="n">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="86">
@@ -85228,13 +85229,55 @@
         <v>3992</v>
       </c>
       <c r="B86" t="n">
-        <v>4.7</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>4.7</v>
+        <v>4.800000000000001</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="8" t="n">
+        <v>1154</v>
+      </c>
+      <c r="B87" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="8" t="n">
+        <v>1541</v>
+      </c>
+      <c r="B88" t="n">
+        <v>4.600000000000001</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>4.600000000000001</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="8" t="n">
+        <v>2999</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected Viewable windows with action
</commit_message>
<xml_diff>
--- a/Library.xlsx
+++ b/Library.xlsx
@@ -84053,13 +84053,13 @@
         <v>1160</v>
       </c>
       <c r="B2" t="n">
-        <v>6.7</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.7</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -84067,13 +84067,13 @@
         <v>1271</v>
       </c>
       <c r="B3" t="n">
-        <v>5.95</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>5.95</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -84081,13 +84081,13 @@
         <v>1289</v>
       </c>
       <c r="B4" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="5">
@@ -84095,13 +84095,13 @@
         <v>1331</v>
       </c>
       <c r="B5" t="n">
-        <v>6.050000000000001</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6.050000000000001</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -84109,13 +84109,13 @@
         <v>1340</v>
       </c>
       <c r="B6" t="n">
-        <v>8.9</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>8.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -84123,13 +84123,13 @@
         <v>1343</v>
       </c>
       <c r="B7" t="n">
-        <v>3.9</v>
+        <v>3.95</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.9</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="8">
@@ -84137,13 +84137,13 @@
         <v>1370</v>
       </c>
       <c r="B8" t="n">
-        <v>5.5</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.5</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -84151,13 +84151,13 @@
         <v>1394</v>
       </c>
       <c r="B9" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="10">
@@ -84165,13 +84165,13 @@
         <v>1406</v>
       </c>
       <c r="B10" t="n">
-        <v>5.550000000000001</v>
+        <v>5.600000000000001</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.550000000000001</v>
+        <v>5.600000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -84179,13 +84179,13 @@
         <v>1454</v>
       </c>
       <c r="B11" t="n">
-        <v>4.3</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.3</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -84193,13 +84193,13 @@
         <v>1502</v>
       </c>
       <c r="B12" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="13">
@@ -84207,13 +84207,13 @@
         <v>1508</v>
       </c>
       <c r="B13" t="n">
-        <v>8.850000000000001</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>8.850000000000001</v>
+        <v>8.949999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -84221,13 +84221,13 @@
         <v>1553</v>
       </c>
       <c r="B14" t="n">
-        <v>4.5</v>
+        <v>4.55</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4.5</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="15">
@@ -84235,13 +84235,13 @@
         <v>1574</v>
       </c>
       <c r="B15" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="16">
@@ -84249,13 +84249,13 @@
         <v>1577</v>
       </c>
       <c r="B16" t="n">
-        <v>4.5</v>
+        <v>4.55</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.5</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="17">
@@ -84263,13 +84263,13 @@
         <v>1763</v>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="18">
@@ -84277,13 +84277,13 @@
         <v>1787</v>
       </c>
       <c r="B18" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="19">
@@ -84291,13 +84291,13 @@
         <v>1799</v>
       </c>
       <c r="B19" t="n">
-        <v>5.550000000000001</v>
+        <v>5.600000000000001</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.550000000000001</v>
+        <v>5.600000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -84305,13 +84305,13 @@
         <v>1856</v>
       </c>
       <c r="B20" t="n">
-        <v>3.8</v>
+        <v>3.85</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.8</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="21">
@@ -84319,13 +84319,13 @@
         <v>1862</v>
       </c>
       <c r="B21" t="n">
-        <v>6.100000000000001</v>
+        <v>6.15</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6.100000000000001</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="22">
@@ -84333,13 +84333,13 @@
         <v>1940</v>
       </c>
       <c r="B22" t="n">
-        <v>6.45</v>
+        <v>6.5</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6.45</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="23">
@@ -84347,13 +84347,13 @@
         <v>2009</v>
       </c>
       <c r="B23" t="n">
-        <v>6.25</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6.25</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="24">
@@ -84361,13 +84361,13 @@
         <v>2039</v>
       </c>
       <c r="B24" t="n">
-        <v>6.15</v>
+        <v>6.2</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6.15</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="25">
@@ -84375,13 +84375,13 @@
         <v>2090</v>
       </c>
       <c r="B25" t="n">
-        <v>6.300000000000001</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6.300000000000001</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -84389,13 +84389,13 @@
         <v>2141</v>
       </c>
       <c r="B26" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="27">
@@ -84403,13 +84403,13 @@
         <v>2150</v>
       </c>
       <c r="B27" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="28">
@@ -84417,13 +84417,13 @@
         <v>2156</v>
       </c>
       <c r="B28" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="29">
@@ -84431,13 +84431,13 @@
         <v>2162</v>
       </c>
       <c r="B29" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="30">
@@ -84445,13 +84445,13 @@
         <v>2204</v>
       </c>
       <c r="B30" t="n">
-        <v>5.9</v>
+        <v>5.95</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>5.9</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="31">
@@ -84459,13 +84459,13 @@
         <v>2207</v>
       </c>
       <c r="B31" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="32">
@@ -84473,13 +84473,13 @@
         <v>2216</v>
       </c>
       <c r="B32" t="n">
-        <v>6.4</v>
+        <v>6.45</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.4</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="33">
@@ -84487,13 +84487,13 @@
         <v>2237</v>
       </c>
       <c r="B33" t="n">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="34">
@@ -84501,13 +84501,13 @@
         <v>2258</v>
       </c>
       <c r="B34" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="35">
@@ -84515,13 +84515,13 @@
         <v>2336</v>
       </c>
       <c r="B35" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="36">
@@ -84529,13 +84529,13 @@
         <v>2363</v>
       </c>
       <c r="B36" t="n">
-        <v>5.9</v>
+        <v>5.95</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>5.9</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="37">
@@ -84543,13 +84543,13 @@
         <v>2402</v>
       </c>
       <c r="B37" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="38">
@@ -84557,13 +84557,13 @@
         <v>2498</v>
       </c>
       <c r="B38" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="39">
@@ -84571,13 +84571,13 @@
         <v>2543</v>
       </c>
       <c r="B39" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="40">
@@ -84585,13 +84585,13 @@
         <v>2639</v>
       </c>
       <c r="B40" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="41">
@@ -84599,13 +84599,13 @@
         <v>2651</v>
       </c>
       <c r="B41" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="42">
@@ -84613,13 +84613,13 @@
         <v>2657</v>
       </c>
       <c r="B42" t="n">
-        <v>4.95</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>4.95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -84627,13 +84627,13 @@
         <v>2747</v>
       </c>
       <c r="B43" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="44">
@@ -84641,13 +84641,13 @@
         <v>2798</v>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -84655,13 +84655,13 @@
         <v>2819</v>
       </c>
       <c r="B45" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>5.100000000000001</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="46">
@@ -84669,13 +84669,13 @@
         <v>2951</v>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>5</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -84683,13 +84683,13 @@
         <v>2972</v>
       </c>
       <c r="B47" t="n">
-        <v>4.600000000000001</v>
+        <v>4.65</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.600000000000001</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="48">
@@ -84697,13 +84697,13 @@
         <v>2975</v>
       </c>
       <c r="B48" t="n">
-        <v>10</v>
+        <v>10.15</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>10</v>
+        <v>10.15</v>
       </c>
     </row>
     <row r="49">
@@ -84711,13 +84711,13 @@
         <v>2990</v>
       </c>
       <c r="B49" t="n">
-        <v>4.45</v>
+        <v>4.5</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4.45</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="50">
@@ -84725,13 +84725,13 @@
         <v>3053</v>
       </c>
       <c r="B50" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="51">
@@ -84739,13 +84739,13 @@
         <v>3074</v>
       </c>
       <c r="B51" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="52">
@@ -84753,13 +84753,13 @@
         <v>3104</v>
       </c>
       <c r="B52" t="n">
-        <v>4.7</v>
+        <v>4.75</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>4.7</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="53">
@@ -84767,13 +84767,13 @@
         <v>3146</v>
       </c>
       <c r="B53" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>5.65</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="54">
@@ -84781,13 +84781,13 @@
         <v>3230</v>
       </c>
       <c r="B54" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="55">
@@ -84795,13 +84795,13 @@
         <v>3242</v>
       </c>
       <c r="B55" t="n">
-        <v>4.800000000000001</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.800000000000001</v>
+        <v>4.850000000000001</v>
       </c>
     </row>
     <row r="56">
@@ -84809,13 +84809,13 @@
         <v>3245</v>
       </c>
       <c r="B56" t="n">
-        <v>6.4</v>
+        <v>6.45</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6.4</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="57">
@@ -84823,13 +84823,13 @@
         <v>3269</v>
       </c>
       <c r="B57" t="n">
-        <v>4.9</v>
+        <v>4.95</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>4.9</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="58">
@@ -84837,13 +84837,13 @@
         <v>3362</v>
       </c>
       <c r="B58" t="n">
-        <v>4.4</v>
+        <v>4.45</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>4.4</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="59">
@@ -84851,13 +84851,13 @@
         <v>3479</v>
       </c>
       <c r="B59" t="n">
-        <v>4.850000000000001</v>
+        <v>4.9</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4.850000000000001</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="60">
@@ -84865,13 +84865,13 @@
         <v>3503</v>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="61">
@@ -84879,13 +84879,13 @@
         <v>3539</v>
       </c>
       <c r="B61" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="62">
@@ -84893,13 +84893,13 @@
         <v>3608</v>
       </c>
       <c r="B62" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>5.850000000000001</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="63">
@@ -84907,13 +84907,13 @@
         <v>3647</v>
       </c>
       <c r="B63" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="64">
@@ -84921,13 +84921,13 @@
         <v>3653</v>
       </c>
       <c r="B64" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="65">
@@ -84935,13 +84935,13 @@
         <v>3671</v>
       </c>
       <c r="B65" t="n">
-        <v>5.050000000000001</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>5.050000000000001</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="66">
@@ -84949,13 +84949,13 @@
         <v>3680</v>
       </c>
       <c r="B66" t="n">
-        <v>3.9</v>
+        <v>3.95</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3.9</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="67">
@@ -84963,13 +84963,13 @@
         <v>3683</v>
       </c>
       <c r="B67" t="n">
-        <v>6.300000000000001</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>6.300000000000001</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="68">
@@ -84977,13 +84977,13 @@
         <v>3722</v>
       </c>
       <c r="B68" t="n">
-        <v>4.2</v>
+        <v>4.25</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>4.2</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="69">
@@ -84991,13 +84991,13 @@
         <v>3728</v>
       </c>
       <c r="B69" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="70">
@@ -85005,13 +85005,13 @@
         <v>3749</v>
       </c>
       <c r="B70" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="71">
@@ -85019,13 +85019,13 @@
         <v>3773</v>
       </c>
       <c r="B71" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>4.100000000000001</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="72">
@@ -85033,13 +85033,13 @@
         <v>3794</v>
       </c>
       <c r="B72" t="n">
-        <v>3.65</v>
+        <v>3.7</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>3.65</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="73">
@@ -85047,13 +85047,13 @@
         <v>3800</v>
       </c>
       <c r="B73" t="n">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="74">
@@ -85061,13 +85061,13 @@
         <v>3803</v>
       </c>
       <c r="B74" t="n">
-        <v>3.65</v>
+        <v>3.7</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3.65</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="75">
@@ -85075,13 +85075,13 @@
         <v>3821</v>
       </c>
       <c r="B75" t="n">
-        <v>5.95</v>
+        <v>6</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>5.95</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -85089,13 +85089,13 @@
         <v>3824</v>
       </c>
       <c r="B76" t="n">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="77">
@@ -85103,13 +85103,13 @@
         <v>3866</v>
       </c>
       <c r="B77" t="n">
-        <v>6.25</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>6.25</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="78">
@@ -85117,13 +85117,13 @@
         <v>3923</v>
       </c>
       <c r="B78" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>6.350000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="79">
@@ -85131,13 +85131,13 @@
         <v>3932</v>
       </c>
       <c r="B79" t="n">
-        <v>4.350000000000001</v>
+        <v>4.4</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>4.350000000000001</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="80">
@@ -85145,13 +85145,13 @@
         <v>3959</v>
       </c>
       <c r="B80" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>5.2</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="81">
@@ -85159,13 +85159,13 @@
         <v>3968</v>
       </c>
       <c r="B81" t="n">
-        <v>6.050000000000001</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>6.050000000000001</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="82">
@@ -85173,13 +85173,13 @@
         <v>3977</v>
       </c>
       <c r="B82" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>4.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="83">
@@ -85187,13 +85187,13 @@
         <v>3980</v>
       </c>
       <c r="B83" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>5.45</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="84">
@@ -85201,13 +85201,13 @@
         <v>3986</v>
       </c>
       <c r="B84" t="n">
-        <v>4.600000000000001</v>
+        <v>4.65</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>4.600000000000001</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="85">
@@ -85215,13 +85215,13 @@
         <v>3989</v>
       </c>
       <c r="B85" t="n">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="86">
@@ -85229,13 +85229,13 @@
         <v>3992</v>
       </c>
       <c r="B86" t="n">
-        <v>4.800000000000001</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>4.800000000000001</v>
+        <v>4.850000000000001</v>
       </c>
     </row>
     <row r="87">
@@ -85243,13 +85243,13 @@
         <v>1154</v>
       </c>
       <c r="B87" t="n">
-        <v>6.9</v>
+        <v>7.050000000000001</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>6.9</v>
+        <v>7.050000000000001</v>
       </c>
     </row>
     <row r="88">
@@ -85257,13 +85257,13 @@
         <v>1541</v>
       </c>
       <c r="B88" t="n">
-        <v>4.600000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>4.600000000000001</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="89">
@@ -85271,13 +85271,13 @@
         <v>2999</v>
       </c>
       <c r="B89" t="n">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corercted Dataframe Return -> to string for GUI
</commit_message>
<xml_diff>
--- a/Library.xlsx
+++ b/Library.xlsx
@@ -24,10 +24,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -82193,7 +82192,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="n"/>
+      <c r="A3" s="11" t="n"/>
       <c r="B3" s="8" t="n">
         <v>1192</v>
       </c>
@@ -82210,7 +82209,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="n"/>
+      <c r="A4" s="12" t="n"/>
       <c r="B4" s="8" t="n">
         <v>1399</v>
       </c>
@@ -82246,7 +82245,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="n"/>
+      <c r="A6" s="12" t="n"/>
       <c r="B6" s="8" t="n">
         <v>3220</v>
       </c>
@@ -82339,7 +82338,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="n"/>
+      <c r="A11" s="12" t="n"/>
       <c r="B11" s="8" t="n">
         <v>511</v>
       </c>
@@ -82489,7 +82488,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="n"/>
+      <c r="A19" s="12" t="n"/>
       <c r="B19" s="8" t="n">
         <v>2098</v>
       </c>
@@ -82525,7 +82524,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="n"/>
+      <c r="A21" s="12" t="n"/>
       <c r="B21" s="8" t="n">
         <v>859</v>
       </c>
@@ -83207,7 +83206,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="8" t="n"/>
+      <c r="A57" s="11" t="n"/>
       <c r="B57" s="8" t="n">
         <v>2827</v>
       </c>
@@ -83224,7 +83223,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="8" t="n"/>
+      <c r="A58" s="12" t="n"/>
       <c r="B58" s="8" t="n">
         <v>766</v>
       </c>
@@ -83963,7 +83962,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="8" t="n"/>
+      <c r="A97" s="12" t="n"/>
       <c r="B97" s="8" t="n">
         <v>2842</v>
       </c>
@@ -84053,13 +84052,13 @@
         <v>1160</v>
       </c>
       <c r="B2" t="n">
-        <v>6.800000000000001</v>
+        <v>7.600000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.800000000000001</v>
+        <v>7.600000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -84067,13 +84066,13 @@
         <v>1271</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="4">
@@ -84081,13 +84080,13 @@
         <v>1289</v>
       </c>
       <c r="B4" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -84095,13 +84094,13 @@
         <v>1331</v>
       </c>
       <c r="B5" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6">
@@ -84109,13 +84108,13 @@
         <v>1340</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -84123,13 +84122,13 @@
         <v>1343</v>
       </c>
       <c r="B7" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -84137,13 +84136,13 @@
         <v>1370</v>
       </c>
       <c r="B8" t="n">
-        <v>5.550000000000001</v>
+        <v>5.95</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.550000000000001</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="9">
@@ -84151,13 +84150,13 @@
         <v>1394</v>
       </c>
       <c r="B9" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -84165,13 +84164,13 @@
         <v>1406</v>
       </c>
       <c r="B10" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -84179,13 +84178,13 @@
         <v>1454</v>
       </c>
       <c r="B11" t="n">
-        <v>4.350000000000001</v>
+        <v>4.75</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.350000000000001</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="12">
@@ -84193,13 +84192,13 @@
         <v>1502</v>
       </c>
       <c r="B12" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -84207,13 +84206,13 @@
         <v>1508</v>
       </c>
       <c r="B13" t="n">
-        <v>8.949999999999999</v>
+        <v>9.75</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>8.949999999999999</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="14">
@@ -84221,13 +84220,13 @@
         <v>1553</v>
       </c>
       <c r="B14" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="15">
@@ -84235,13 +84234,13 @@
         <v>1574</v>
       </c>
       <c r="B15" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="16">
@@ -84249,13 +84248,13 @@
         <v>1577</v>
       </c>
       <c r="B16" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="17">
@@ -84263,13 +84262,13 @@
         <v>1763</v>
       </c>
       <c r="B17" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="18">
@@ -84277,13 +84276,13 @@
         <v>1787</v>
       </c>
       <c r="B18" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="19">
@@ -84291,13 +84290,13 @@
         <v>1799</v>
       </c>
       <c r="B19" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -84305,13 +84304,13 @@
         <v>1856</v>
       </c>
       <c r="B20" t="n">
-        <v>3.85</v>
+        <v>4.25</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.85</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="21">
@@ -84319,13 +84318,13 @@
         <v>1862</v>
       </c>
       <c r="B21" t="n">
-        <v>6.15</v>
+        <v>6.550000000000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6.15</v>
+        <v>6.550000000000001</v>
       </c>
     </row>
     <row r="22">
@@ -84333,13 +84332,13 @@
         <v>1940</v>
       </c>
       <c r="B22" t="n">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="23">
@@ -84347,13 +84346,13 @@
         <v>2009</v>
       </c>
       <c r="B23" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="24">
@@ -84361,13 +84360,13 @@
         <v>2039</v>
       </c>
       <c r="B24" t="n">
-        <v>6.2</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6.2</v>
+        <v>6.600000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -84375,13 +84374,13 @@
         <v>2090</v>
       </c>
       <c r="B25" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="26">
@@ -84389,13 +84388,13 @@
         <v>2141</v>
       </c>
       <c r="B26" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -84403,13 +84402,13 @@
         <v>2150</v>
       </c>
       <c r="B27" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="28">
@@ -84417,13 +84416,13 @@
         <v>2156</v>
       </c>
       <c r="B28" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="29">
@@ -84431,13 +84430,13 @@
         <v>2162</v>
       </c>
       <c r="B29" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="30">
@@ -84445,13 +84444,13 @@
         <v>2204</v>
       </c>
       <c r="B30" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -84459,13 +84458,13 @@
         <v>2207</v>
       </c>
       <c r="B31" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -84473,13 +84472,13 @@
         <v>2216</v>
       </c>
       <c r="B32" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -84487,13 +84486,13 @@
         <v>2237</v>
       </c>
       <c r="B33" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="34">
@@ -84501,13 +84500,13 @@
         <v>2258</v>
       </c>
       <c r="B34" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="35">
@@ -84515,13 +84514,13 @@
         <v>2336</v>
       </c>
       <c r="B35" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="36">
@@ -84529,13 +84528,13 @@
         <v>2363</v>
       </c>
       <c r="B36" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="37">
@@ -84543,13 +84542,13 @@
         <v>2402</v>
       </c>
       <c r="B37" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="38">
@@ -84557,13 +84556,13 @@
         <v>2498</v>
       </c>
       <c r="B38" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="39">
@@ -84571,13 +84570,13 @@
         <v>2543</v>
       </c>
       <c r="B39" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -84585,13 +84584,13 @@
         <v>2639</v>
       </c>
       <c r="B40" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="41">
@@ -84599,13 +84598,13 @@
         <v>2651</v>
       </c>
       <c r="B41" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="42">
@@ -84613,13 +84612,13 @@
         <v>2657</v>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="43">
@@ -84627,13 +84626,13 @@
         <v>2747</v>
       </c>
       <c r="B43" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -84641,13 +84640,13 @@
         <v>2798</v>
       </c>
       <c r="B44" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="45">
@@ -84655,13 +84654,13 @@
         <v>2819</v>
       </c>
       <c r="B45" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="46">
@@ -84669,13 +84668,13 @@
         <v>2951</v>
       </c>
       <c r="B46" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="47">
@@ -84683,13 +84682,13 @@
         <v>2972</v>
       </c>
       <c r="B47" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="48">
@@ -84697,13 +84696,13 @@
         <v>2975</v>
       </c>
       <c r="B48" t="n">
-        <v>10.15</v>
+        <v>11.35</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>10.15</v>
+        <v>11.35</v>
       </c>
     </row>
     <row r="49">
@@ -84711,13 +84710,13 @@
         <v>2990</v>
       </c>
       <c r="B49" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="50">
@@ -84725,13 +84724,13 @@
         <v>3053</v>
       </c>
       <c r="B50" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="51">
@@ -84739,13 +84738,13 @@
         <v>3074</v>
       </c>
       <c r="B51" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -84753,13 +84752,13 @@
         <v>3104</v>
       </c>
       <c r="B52" t="n">
-        <v>4.75</v>
+        <v>5.15</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>4.75</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="53">
@@ -84767,13 +84766,13 @@
         <v>3146</v>
       </c>
       <c r="B53" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="54">
@@ -84781,13 +84780,13 @@
         <v>3230</v>
       </c>
       <c r="B54" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="55">
@@ -84795,13 +84794,13 @@
         <v>3242</v>
       </c>
       <c r="B55" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="56">
@@ -84809,13 +84808,13 @@
         <v>3245</v>
       </c>
       <c r="B56" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
     </row>
     <row r="57">
@@ -84823,13 +84822,13 @@
         <v>3269</v>
       </c>
       <c r="B57" t="n">
-        <v>4.95</v>
+        <v>5.350000000000001</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>4.95</v>
+        <v>5.350000000000001</v>
       </c>
     </row>
     <row r="58">
@@ -84837,13 +84836,13 @@
         <v>3362</v>
       </c>
       <c r="B58" t="n">
-        <v>4.45</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>4.45</v>
+        <v>4.850000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -84851,13 +84850,13 @@
         <v>3479</v>
       </c>
       <c r="B59" t="n">
-        <v>4.9</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4.9</v>
+        <v>5.300000000000001</v>
       </c>
     </row>
     <row r="60">
@@ -84865,13 +84864,13 @@
         <v>3503</v>
       </c>
       <c r="B60" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="61">
@@ -84879,13 +84878,13 @@
         <v>3539</v>
       </c>
       <c r="B61" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="62">
@@ -84893,13 +84892,13 @@
         <v>3608</v>
       </c>
       <c r="B62" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="63">
@@ -84907,13 +84906,13 @@
         <v>3647</v>
       </c>
       <c r="B63" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="64">
@@ -84921,13 +84920,13 @@
         <v>3653</v>
       </c>
       <c r="B64" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="65">
@@ -84935,13 +84934,13 @@
         <v>3671</v>
       </c>
       <c r="B65" t="n">
-        <v>5.100000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>5.100000000000001</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="66">
@@ -84949,13 +84948,13 @@
         <v>3680</v>
       </c>
       <c r="B66" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="67">
@@ -84963,13 +84962,13 @@
         <v>3683</v>
       </c>
       <c r="B67" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="68">
@@ -84977,13 +84976,13 @@
         <v>3722</v>
       </c>
       <c r="B68" t="n">
-        <v>4.25</v>
+        <v>4.65</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>4.25</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="69">
@@ -84991,13 +84990,13 @@
         <v>3728</v>
       </c>
       <c r="B69" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="70">
@@ -85005,13 +85004,13 @@
         <v>3749</v>
       </c>
       <c r="B70" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="71">
@@ -85019,13 +85018,13 @@
         <v>3773</v>
       </c>
       <c r="B71" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="72">
@@ -85033,13 +85032,13 @@
         <v>3794</v>
       </c>
       <c r="B72" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -85047,13 +85046,13 @@
         <v>3800</v>
       </c>
       <c r="B73" t="n">
-        <v>3.25</v>
+        <v>3.65</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>3.25</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="74">
@@ -85061,13 +85060,13 @@
         <v>3803</v>
       </c>
       <c r="B74" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="75">
@@ -85075,13 +85074,13 @@
         <v>3821</v>
       </c>
       <c r="B75" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="76">
@@ -85089,13 +85088,13 @@
         <v>3824</v>
       </c>
       <c r="B76" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="77">
@@ -85103,13 +85102,13 @@
         <v>3866</v>
       </c>
       <c r="B77" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="78">
@@ -85117,13 +85116,13 @@
         <v>3923</v>
       </c>
       <c r="B78" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -85131,13 +85130,13 @@
         <v>3932</v>
       </c>
       <c r="B79" t="n">
-        <v>4.4</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>4.4</v>
+        <v>4.800000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -85145,13 +85144,13 @@
         <v>3959</v>
       </c>
       <c r="B80" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="81">
@@ -85159,13 +85158,13 @@
         <v>3968</v>
       </c>
       <c r="B81" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="82">
@@ -85173,13 +85172,13 @@
         <v>3977</v>
       </c>
       <c r="B82" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="83">
@@ -85187,13 +85186,13 @@
         <v>3980</v>
       </c>
       <c r="B83" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="84">
@@ -85201,13 +85200,13 @@
         <v>3986</v>
       </c>
       <c r="B84" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -85215,13 +85214,13 @@
         <v>3989</v>
       </c>
       <c r="B85" t="n">
-        <v>6.5</v>
+        <v>7.300000000000001</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>6.5</v>
+        <v>7.300000000000001</v>
       </c>
     </row>
     <row r="86">
@@ -85229,13 +85228,13 @@
         <v>3992</v>
       </c>
       <c r="B86" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="87">
@@ -85243,13 +85242,13 @@
         <v>1154</v>
       </c>
       <c r="B87" t="n">
-        <v>7.050000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>7.050000000000001</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="88">
@@ -85257,13 +85256,13 @@
         <v>1541</v>
       </c>
       <c r="B88" t="n">
-        <v>4.7</v>
+        <v>5.5</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>4.7</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="89">
@@ -85271,13 +85270,13 @@
         <v>2999</v>
       </c>
       <c r="B89" t="n">
-        <v>2.95</v>
+        <v>3.35</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>2.95</v>
+        <v>3.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all backend comments and adjustments
</commit_message>
<xml_diff>
--- a/Library.xlsx
+++ b/Library.xlsx
@@ -24,10 +24,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -82193,7 +82192,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="n"/>
+      <c r="A3" s="11" t="n"/>
       <c r="B3" s="8" t="n">
         <v>1192</v>
       </c>
@@ -82210,7 +82209,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="n"/>
+      <c r="A4" s="12" t="n"/>
       <c r="B4" s="8" t="n">
         <v>1399</v>
       </c>
@@ -82246,7 +82245,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="n"/>
+      <c r="A6" s="12" t="n"/>
       <c r="B6" s="8" t="n">
         <v>3220</v>
       </c>
@@ -82339,7 +82338,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="n"/>
+      <c r="A11" s="12" t="n"/>
       <c r="B11" s="8" t="n">
         <v>511</v>
       </c>
@@ -82489,7 +82488,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="n"/>
+      <c r="A19" s="12" t="n"/>
       <c r="B19" s="8" t="n">
         <v>2098</v>
       </c>
@@ -82525,7 +82524,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="n"/>
+      <c r="A21" s="12" t="n"/>
       <c r="B21" s="8" t="n">
         <v>859</v>
       </c>
@@ -83207,7 +83206,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="8" t="n"/>
+      <c r="A57" s="11" t="n"/>
       <c r="B57" s="8" t="n">
         <v>2827</v>
       </c>
@@ -83224,7 +83223,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="8" t="n"/>
+      <c r="A58" s="12" t="n"/>
       <c r="B58" s="8" t="n">
         <v>766</v>
       </c>
@@ -83963,7 +83962,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="8" t="n"/>
+      <c r="A97" s="12" t="n"/>
       <c r="B97" s="8" t="n">
         <v>2842</v>
       </c>
@@ -84053,13 +84052,13 @@
         <v>1160</v>
       </c>
       <c r="B2" t="n">
-        <v>6.800000000000001</v>
+        <v>7.600000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.800000000000001</v>
+        <v>7.600000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -84067,13 +84066,13 @@
         <v>1271</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="4">
@@ -84081,13 +84080,13 @@
         <v>1289</v>
       </c>
       <c r="B4" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -84095,13 +84094,13 @@
         <v>1331</v>
       </c>
       <c r="B5" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6">
@@ -84109,13 +84108,13 @@
         <v>1340</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -84123,13 +84122,13 @@
         <v>1343</v>
       </c>
       <c r="B7" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -84137,13 +84136,13 @@
         <v>1370</v>
       </c>
       <c r="B8" t="n">
-        <v>5.550000000000001</v>
+        <v>5.95</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.550000000000001</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="9">
@@ -84151,13 +84150,13 @@
         <v>1394</v>
       </c>
       <c r="B9" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -84165,13 +84164,13 @@
         <v>1406</v>
       </c>
       <c r="B10" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -84179,13 +84178,13 @@
         <v>1454</v>
       </c>
       <c r="B11" t="n">
-        <v>4.350000000000001</v>
+        <v>4.75</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.350000000000001</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="12">
@@ -84193,13 +84192,13 @@
         <v>1502</v>
       </c>
       <c r="B12" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -84207,13 +84206,13 @@
         <v>1508</v>
       </c>
       <c r="B13" t="n">
-        <v>8.949999999999999</v>
+        <v>9.75</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>8.949999999999999</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="14">
@@ -84221,13 +84220,13 @@
         <v>1553</v>
       </c>
       <c r="B14" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="15">
@@ -84235,13 +84234,13 @@
         <v>1574</v>
       </c>
       <c r="B15" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="16">
@@ -84249,13 +84248,13 @@
         <v>1577</v>
       </c>
       <c r="B16" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.55</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="17">
@@ -84263,13 +84262,13 @@
         <v>1763</v>
       </c>
       <c r="B17" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="18">
@@ -84277,13 +84276,13 @@
         <v>1787</v>
       </c>
       <c r="B18" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="19">
@@ -84291,13 +84290,13 @@
         <v>1799</v>
       </c>
       <c r="B19" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.600000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -84305,13 +84304,13 @@
         <v>1856</v>
       </c>
       <c r="B20" t="n">
-        <v>3.85</v>
+        <v>4.25</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.85</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="21">
@@ -84319,13 +84318,13 @@
         <v>1862</v>
       </c>
       <c r="B21" t="n">
-        <v>6.15</v>
+        <v>6.550000000000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6.15</v>
+        <v>6.550000000000001</v>
       </c>
     </row>
     <row r="22">
@@ -84333,13 +84332,13 @@
         <v>1940</v>
       </c>
       <c r="B22" t="n">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="23">
@@ -84347,13 +84346,13 @@
         <v>2009</v>
       </c>
       <c r="B23" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="24">
@@ -84361,13 +84360,13 @@
         <v>2039</v>
       </c>
       <c r="B24" t="n">
-        <v>6.2</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6.2</v>
+        <v>6.600000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -84375,13 +84374,13 @@
         <v>2090</v>
       </c>
       <c r="B25" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="26">
@@ -84389,13 +84388,13 @@
         <v>2141</v>
       </c>
       <c r="B26" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -84403,13 +84402,13 @@
         <v>2150</v>
       </c>
       <c r="B27" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="28">
@@ -84417,13 +84416,13 @@
         <v>2156</v>
       </c>
       <c r="B28" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="29">
@@ -84431,13 +84430,13 @@
         <v>2162</v>
       </c>
       <c r="B29" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="30">
@@ -84445,13 +84444,13 @@
         <v>2204</v>
       </c>
       <c r="B30" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -84459,13 +84458,13 @@
         <v>2207</v>
       </c>
       <c r="B31" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -84473,13 +84472,13 @@
         <v>2216</v>
       </c>
       <c r="B32" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -84487,13 +84486,13 @@
         <v>2237</v>
       </c>
       <c r="B33" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="34">
@@ -84501,13 +84500,13 @@
         <v>2258</v>
       </c>
       <c r="B34" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="35">
@@ -84515,13 +84514,13 @@
         <v>2336</v>
       </c>
       <c r="B35" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="36">
@@ -84529,13 +84528,13 @@
         <v>2363</v>
       </c>
       <c r="B36" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>5.95</v>
+        <v>6.350000000000001</v>
       </c>
     </row>
     <row r="37">
@@ -84543,13 +84542,13 @@
         <v>2402</v>
       </c>
       <c r="B37" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="38">
@@ -84557,13 +84556,13 @@
         <v>2498</v>
       </c>
       <c r="B38" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="39">
@@ -84571,13 +84570,13 @@
         <v>2543</v>
       </c>
       <c r="B39" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -84585,13 +84584,13 @@
         <v>2639</v>
       </c>
       <c r="B40" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="41">
@@ -84599,13 +84598,13 @@
         <v>2651</v>
       </c>
       <c r="B41" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="42">
@@ -84613,13 +84612,13 @@
         <v>2657</v>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="43">
@@ -84627,13 +84626,13 @@
         <v>2747</v>
       </c>
       <c r="B43" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -84641,13 +84640,13 @@
         <v>2798</v>
       </c>
       <c r="B44" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="45">
@@ -84655,13 +84654,13 @@
         <v>2819</v>
       </c>
       <c r="B45" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>5.15</v>
+        <v>5.550000000000001</v>
       </c>
     </row>
     <row r="46">
@@ -84669,13 +84668,13 @@
         <v>2951</v>
       </c>
       <c r="B46" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>5.050000000000001</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="47">
@@ -84683,13 +84682,13 @@
         <v>2972</v>
       </c>
       <c r="B47" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="48">
@@ -84697,13 +84696,13 @@
         <v>2975</v>
       </c>
       <c r="B48" t="n">
-        <v>10.15</v>
+        <v>11.35</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>10.15</v>
+        <v>11.35</v>
       </c>
     </row>
     <row r="49">
@@ -84711,13 +84710,13 @@
         <v>2990</v>
       </c>
       <c r="B49" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="50">
@@ -84725,13 +84724,13 @@
         <v>3053</v>
       </c>
       <c r="B50" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="51">
@@ -84739,13 +84738,13 @@
         <v>3074</v>
       </c>
       <c r="B51" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -84753,13 +84752,13 @@
         <v>3104</v>
       </c>
       <c r="B52" t="n">
-        <v>4.75</v>
+        <v>5.15</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>4.75</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="53">
@@ -84767,13 +84766,13 @@
         <v>3146</v>
       </c>
       <c r="B53" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>5.7</v>
+        <v>6.100000000000001</v>
       </c>
     </row>
     <row r="54">
@@ -84781,13 +84780,13 @@
         <v>3230</v>
       </c>
       <c r="B54" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>3.75</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="55">
@@ -84795,13 +84794,13 @@
         <v>3242</v>
       </c>
       <c r="B55" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="56">
@@ -84809,13 +84808,13 @@
         <v>3245</v>
       </c>
       <c r="B56" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6.45</v>
+        <v>6.850000000000001</v>
       </c>
     </row>
     <row r="57">
@@ -84823,13 +84822,13 @@
         <v>3269</v>
       </c>
       <c r="B57" t="n">
-        <v>4.95</v>
+        <v>5.350000000000001</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>4.95</v>
+        <v>5.350000000000001</v>
       </c>
     </row>
     <row r="58">
@@ -84837,13 +84836,13 @@
         <v>3362</v>
       </c>
       <c r="B58" t="n">
-        <v>4.45</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>4.45</v>
+        <v>4.850000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -84851,13 +84850,13 @@
         <v>3479</v>
       </c>
       <c r="B59" t="n">
-        <v>4.9</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4.9</v>
+        <v>5.300000000000001</v>
       </c>
     </row>
     <row r="60">
@@ -84865,13 +84864,13 @@
         <v>3503</v>
       </c>
       <c r="B60" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="61">
@@ -84879,13 +84878,13 @@
         <v>3539</v>
       </c>
       <c r="B61" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="62">
@@ -84893,13 +84892,13 @@
         <v>3608</v>
       </c>
       <c r="B62" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>5.9</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
     <row r="63">
@@ -84907,13 +84906,13 @@
         <v>3647</v>
       </c>
       <c r="B63" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="64">
@@ -84921,13 +84920,13 @@
         <v>3653</v>
       </c>
       <c r="B64" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="65">
@@ -84935,13 +84934,13 @@
         <v>3671</v>
       </c>
       <c r="B65" t="n">
-        <v>5.100000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>5.100000000000001</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="66">
@@ -84949,13 +84948,13 @@
         <v>3680</v>
       </c>
       <c r="B66" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3.95</v>
+        <v>4.350000000000001</v>
       </c>
     </row>
     <row r="67">
@@ -84963,13 +84962,13 @@
         <v>3683</v>
       </c>
       <c r="B67" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>6.350000000000001</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="68">
@@ -84977,13 +84976,13 @@
         <v>3722</v>
       </c>
       <c r="B68" t="n">
-        <v>4.25</v>
+        <v>4.65</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>4.25</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="69">
@@ -84991,13 +84990,13 @@
         <v>3728</v>
       </c>
       <c r="B69" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="70">
@@ -85005,13 +85004,13 @@
         <v>3749</v>
       </c>
       <c r="B70" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>4.05</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="71">
@@ -85019,13 +85018,13 @@
         <v>3773</v>
       </c>
       <c r="B71" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>4.15</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="72">
@@ -85033,13 +85032,13 @@
         <v>3794</v>
       </c>
       <c r="B72" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -85047,13 +85046,13 @@
         <v>3800</v>
       </c>
       <c r="B73" t="n">
-        <v>3.25</v>
+        <v>3.65</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>3.25</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="74">
@@ -85061,13 +85060,13 @@
         <v>3803</v>
       </c>
       <c r="B74" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3.7</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="75">
@@ -85075,13 +85074,13 @@
         <v>3821</v>
       </c>
       <c r="B75" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="76">
@@ -85089,13 +85088,13 @@
         <v>3824</v>
       </c>
       <c r="B76" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="77">
@@ -85103,13 +85102,13 @@
         <v>3866</v>
       </c>
       <c r="B77" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>6.300000000000001</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="78">
@@ -85117,13 +85116,13 @@
         <v>3923</v>
       </c>
       <c r="B78" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>6.4</v>
+        <v>6.800000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -85131,13 +85130,13 @@
         <v>3932</v>
       </c>
       <c r="B79" t="n">
-        <v>4.4</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>4.4</v>
+        <v>4.800000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -85145,13 +85144,13 @@
         <v>3959</v>
       </c>
       <c r="B80" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>5.25</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="81">
@@ -85159,13 +85158,13 @@
         <v>3968</v>
       </c>
       <c r="B81" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>6.100000000000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="82">
@@ -85173,13 +85172,13 @@
         <v>3977</v>
       </c>
       <c r="B82" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>4.7</v>
+        <v>5.100000000000001</v>
       </c>
     </row>
     <row r="83">
@@ -85187,13 +85186,13 @@
         <v>3980</v>
       </c>
       <c r="B83" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="84">
@@ -85201,13 +85200,13 @@
         <v>3986</v>
       </c>
       <c r="B84" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>4.65</v>
+        <v>5.050000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -85215,13 +85214,13 @@
         <v>3989</v>
       </c>
       <c r="B85" t="n">
-        <v>6.5</v>
+        <v>7.300000000000001</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>6.5</v>
+        <v>7.300000000000001</v>
       </c>
     </row>
     <row r="86">
@@ -85229,13 +85228,13 @@
         <v>3992</v>
       </c>
       <c r="B86" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>4.850000000000001</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="87">
@@ -85243,13 +85242,13 @@
         <v>1154</v>
       </c>
       <c r="B87" t="n">
-        <v>7.050000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>7.050000000000001</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="88">
@@ -85257,13 +85256,13 @@
         <v>1541</v>
       </c>
       <c r="B88" t="n">
-        <v>4.7</v>
+        <v>5.5</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>4.7</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="89">
@@ -85271,13 +85270,13 @@
         <v>2999</v>
       </c>
       <c r="B89" t="n">
-        <v>2.95</v>
+        <v>3.35</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>2.95</v>
+        <v>3.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>